<commit_message>
JP-1481: Support "allow web login" for create/edit user
</commit_message>
<xml_diff>
--- a/Workbooks/JA/アセット.xlsx
+++ b/Workbooks/JA/アセット.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryota.okuji\Documents\UiPath\OrchestratorManager\Workbooks\JA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C769E9-B449-491D-A67F-5E3EAE17A28E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA33D23F-E3A0-4F19-A52D-7678DB84BD87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6390" yWindow="1880" windowWidth="29640" windowHeight="15630" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="63030" yWindow="690" windowWidth="28800" windowHeight="11265" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="取得" sheetId="4" r:id="rId1"/>

</xml_diff>

<commit_message>
JP1472: Support directory user creation
</commit_message>
<xml_diff>
--- a/Workbooks/JA/アセット.xlsx
+++ b/Workbooks/JA/アセット.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryota.okuji\Documents\UiPath\OrchestratorManager\Workbooks\JA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA33D23F-E3A0-4F19-A52D-7678DB84BD87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB42C248-7DE3-42CB-849A-F0D9D722B21F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="63030" yWindow="690" windowWidth="28800" windowHeight="11265" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4940" yWindow="4940" windowWidth="28800" windowHeight="15460" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="取得" sheetId="4" r:id="rId1"/>
@@ -2319,6 +2319,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2B90804-4CC2-4F3A-A5A0-B313E9BACDDF}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4600,6 +4601,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6344F8B8-E12C-4A10-9CFE-BCB8BEC8153F}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6873,6 +6875,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:H200"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8930,6 +8933,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56493D34-EA23-4634-A655-5148B0AC19AA}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:H201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10993,6 +10997,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECF20293-3040-451C-BEA0-1DF5FCF14B01}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:E203"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12452,6 +12457,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1257E298-9813-458A-8168-A2A66F15D641}">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:F201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14103,6 +14109,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2A7D921-E601-49D8-BBF5-CB56640085F5}">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:E201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">

</xml_diff>

<commit_message>
Remove unused ExternalJobKey from Trigger xlsx sheets
</commit_message>
<xml_diff>
--- a/Workbooks/JA/アセット.xlsx
+++ b/Workbooks/JA/アセット.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryota.okuji\Documents\UiPath\OrchestratorManager\Workbooks\JA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6411E1D-AC38-461B-B367-52E0F0720133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B93A3A-4DE6-4DC3-A32D-AEE8C9E82A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="61575" yWindow="1260" windowWidth="23640" windowHeight="12630" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60075" yWindow="1200" windowWidth="35190" windowHeight="12660" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="取得" sheetId="4" r:id="rId1"/>

</xml_diff>

<commit_message>
JP-1495: Get Execution Settings when getting Robots from Classic Folders
</commit_message>
<xml_diff>
--- a/Workbooks/JA/アセット.xlsx
+++ b/Workbooks/JA/アセット.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryota.okuji\Documents\UiPath\OrchestratorManager\Workbooks\JA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9136FDE2-CAE2-4DB9-9659-2FAA781E72C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{890E78C3-B36B-4547-B074-323FD1787C3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2940" yWindow="10690" windowWidth="19420" windowHeight="10420" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="取得" sheetId="4" r:id="rId1"/>

</xml_diff>

<commit_message>
Support enabling/disabling AR/UR explicitly using Create/Edit User
</commit_message>
<xml_diff>
--- a/Workbooks/JA/アセット.xlsx
+++ b/Workbooks/JA/アセット.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryota.okuji\Documents\UiPath\OrchestratorManager\Workbooks\JA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16CAAD8-E858-4BBE-8D12-53FC43AF2795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDCC098B-3EE8-441A-8EA6-2D8EC4089DDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8550" yWindow="2430" windowWidth="28800" windowHeight="11385" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5925" yWindow="1335" windowWidth="30510" windowHeight="10200" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="取得" sheetId="4" r:id="rId1"/>

</xml_diff>

<commit_message>
Link Queue to multiple Folders
</commit_message>
<xml_diff>
--- a/Workbooks/JA/アセット.xlsx
+++ b/Workbooks/JA/アセット.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryota.okuji\Documents\UiPath\OrchestratorManager\Workbooks\JA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE2885D-DF37-4B03-A879-84F40450C8FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94BFBC30-6B1C-474D-BB35-5C3E1D8293E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9000" yWindow="1335" windowWidth="28800" windowHeight="11385" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23780" yWindow="9920" windowWidth="19200" windowHeight="4750" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="取得" sheetId="4" r:id="rId1"/>

</xml_diff>